<commit_message>
Fix: Vietnamese PDF font and email attachment filename encoding
</commit_message>
<xml_diff>
--- a/Book data.xlsx
+++ b/Book data.xlsx
@@ -1,87 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10102"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tungnguyen/Desktop/excel_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E35B80-C991-FC4C-8014-93A67B8A7F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630" activeTab="1"/>
+    <workbookView xWindow="1040" yWindow="500" windowWidth="37360" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thông tin" sheetId="1" r:id="rId1"/>
     <sheet name="Lương" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={bed1e275-4b88-4cb5-8a27-6704ead4d86d}</author>
+    <author/>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0" shapeId="0">
+    <comment ref="AM1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
- Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-	Nhờ Loan gửi link cho anh Chương cập nhật thông tin mới để làm HĐ
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
- Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-	Nhờ Loan gửi link cho anh Chương cập nhật thông tin mới để làm HĐ
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-    <author>tc={bed1e275-4b88-4cb5-8a27-6704ead4d86d}</author>
-  </authors>
-  <commentList>
-    <comment ref="AM1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>1% Lương Cơ Bản : Mức đóng đoàn phí tối đa = 10% x Mức lương cơ sở
@@ -90,47 +61,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU1" authorId="0" shapeId="0">
+    <comment ref="AU1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Phí Đoàn Viên + Thu Nhận NLĐ thực nhận + Tổng các khoản phải nộp hàng tháng cho CQNN</t>
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>"Tiền phụ cấp thuê nhà không vượt quá 15% tổng thu nhập chịu thuế TNCN (chưa bao gồm tiền thuê nhà
  Chịu thuế TNCN của 2310000Vnđ/tháng."</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B6" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
- Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-	Nhờ Loan gửi link cho anh Chương cập nhật thông tin mới để làm HĐ
-</t>
         </r>
       </text>
     </comment>
@@ -412,12 +368,6 @@
     <t>THÔNG TIN NHÂN SỰ</t>
   </si>
   <si>
-    <t>btran0712@gmail.com</t>
-  </si>
-  <si>
-    <t>Td90@gmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">HỌ TÊN NHÂN VIÊN </t>
   </si>
   <si>
@@ -460,6 +410,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>Tiền ăn</t>
     </r>
@@ -469,6 +420,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> (miễn thuế TNCN)</t>
     </r>
@@ -483,6 +435,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">Tiền hỗ trợ điện thoại </t>
     </r>
@@ -492,6 +445,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>(miễn thuế TNCN)</t>
     </r>
@@ -515,6 +469,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">Chi phí trang phục / tháng </t>
     </r>
@@ -524,6 +479,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>(miễn thuế TNCN)</t>
     </r>
@@ -707,9 +663,6 @@
     <t>Thiết kế</t>
   </si>
   <si>
-    <t>Ahothanh@gmail.com</t>
-  </si>
-  <si>
     <t>Chuyên Viên Vận Hành và Dữ Liệu Bản Đồ</t>
   </si>
   <si>
@@ -759,13 +712,22 @@
     <t>Ân Hồng C</t>
   </si>
   <si>
-    <t>AnC5599@gmail.com</t>
+    <t>nguyennhattung2104@gmail.com</t>
+  </si>
+  <si>
+    <t>thaonguyentt021@gmail.com</t>
+  </si>
+  <si>
+    <t>kenzopassion2022@gmail.com</t>
+  </si>
+  <si>
+    <t>thaonguyentt7021@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd"/>
   </numFmts>
@@ -782,46 +744,54 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF434343"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <u/>
@@ -837,17 +807,20 @@
       <sz val="10"/>
       <color rgb="FF212529"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="29">
@@ -1266,7 +1239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1292,23 +1265,143 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="19" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="22" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="27" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="14" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="28" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="28" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="19" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="19" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="19" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1330,76 +1423,28 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="19" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="26" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="20" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1428,222 +1473,13 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="25" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="26" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="22" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="27" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="14" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="28" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="28" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="19" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="20" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="12" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="19" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="19" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF999999"/>
@@ -1671,6 +1507,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Thiết lập"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1935,529 +1784,529 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BK9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="49" t="s">
+    <row r="1" spans="1:63" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E1" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
     </row>
-    <row r="3" spans="1:63" s="9" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:63" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="70" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="10" t="s">
+      <c r="I3" s="54"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="S3" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="T3" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="U3" s="14"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="17" t="s">
+      <c r="U3" s="54"/>
+      <c r="V3" s="57"/>
+      <c r="W3" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="X3" s="18" t="s">
+      <c r="X3" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14"/>
-      <c r="AB3" s="15"/>
-      <c r="AC3" s="19" t="s">
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54"/>
+      <c r="AB3" s="57"/>
+      <c r="AC3" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="AD3" s="14"/>
-      <c r="AE3" s="14"/>
-      <c r="AF3" s="14"/>
-      <c r="AG3" s="15"/>
-      <c r="AH3" s="20" t="s">
+      <c r="AD3" s="54"/>
+      <c r="AE3" s="54"/>
+      <c r="AF3" s="54"/>
+      <c r="AG3" s="57"/>
+      <c r="AH3" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="AI3" s="14"/>
-      <c r="AJ3" s="14"/>
-      <c r="AK3" s="14"/>
-      <c r="AL3" s="15"/>
-      <c r="AM3" s="21" t="s">
+      <c r="AI3" s="54"/>
+      <c r="AJ3" s="54"/>
+      <c r="AK3" s="54"/>
+      <c r="AL3" s="57"/>
+      <c r="AM3" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="AN3" s="14"/>
-      <c r="AO3" s="14"/>
-      <c r="AP3" s="14"/>
-      <c r="AQ3" s="15"/>
-      <c r="AR3" s="22" t="s">
+      <c r="AN3" s="54"/>
+      <c r="AO3" s="54"/>
+      <c r="AP3" s="54"/>
+      <c r="AQ3" s="57"/>
+      <c r="AR3" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="AS3" s="23"/>
-      <c r="AT3" s="23"/>
-      <c r="AU3" s="23"/>
-      <c r="AV3" s="23"/>
-      <c r="AW3" s="24"/>
-      <c r="AX3" s="25" t="s">
+      <c r="AS3" s="65"/>
+      <c r="AT3" s="65"/>
+      <c r="AU3" s="65"/>
+      <c r="AV3" s="65"/>
+      <c r="AW3" s="66"/>
+      <c r="AX3" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="AY3" s="26" t="s">
+      <c r="AY3" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="AZ3" s="14"/>
-      <c r="BA3" s="14"/>
-      <c r="BB3" s="14"/>
-      <c r="BC3" s="14"/>
-      <c r="BD3" s="14"/>
-      <c r="BE3" s="27" t="s">
+      <c r="AZ3" s="54"/>
+      <c r="BA3" s="54"/>
+      <c r="BB3" s="54"/>
+      <c r="BC3" s="54"/>
+      <c r="BD3" s="54"/>
+      <c r="BE3" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="BF3" s="28" t="s">
+      <c r="BF3" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="BG3" s="14"/>
-      <c r="BH3" s="14"/>
-      <c r="BI3" s="14"/>
-      <c r="BJ3" s="15"/>
+      <c r="BG3" s="54"/>
+      <c r="BH3" s="54"/>
+      <c r="BI3" s="54"/>
+      <c r="BJ3" s="57"/>
       <c r="BK3" s="8"/>
     </row>
-    <row r="4" spans="1:63" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="30" t="s">
+    <row r="4" spans="1:63" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="52"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="J4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="31" t="s">
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="U4" s="31" t="s">
+      <c r="U4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="V4" s="31" t="s">
+      <c r="V4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="W4" s="29"/>
-      <c r="X4" s="32" t="s">
+      <c r="W4" s="52"/>
+      <c r="X4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="Y4" s="33" t="s">
+      <c r="Y4" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="Z4" s="33" t="s">
+      <c r="Z4" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AA4" s="34" t="s">
+      <c r="AA4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="AB4" s="34" t="s">
+      <c r="AB4" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AC4" s="35" t="s">
+      <c r="AC4" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="AD4" s="35" t="s">
+      <c r="AD4" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="AE4" s="35" t="s">
+      <c r="AE4" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AF4" s="35" t="s">
+      <c r="AF4" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AG4" s="35" t="s">
+      <c r="AG4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="AH4" s="36" t="s">
+      <c r="AH4" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="AI4" s="36" t="s">
+      <c r="AI4" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AJ4" s="36" t="s">
+      <c r="AJ4" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="AK4" s="36" t="s">
+      <c r="AK4" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="AL4" s="36" t="s">
+      <c r="AL4" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="AM4" s="37" t="s">
+      <c r="AM4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="AN4" s="37" t="s">
+      <c r="AN4" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="AO4" s="37" t="s">
+      <c r="AO4" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AP4" s="37" t="s">
+      <c r="AP4" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="AQ4" s="37" t="s">
+      <c r="AQ4" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="AR4" s="38"/>
-      <c r="AS4" s="39"/>
-      <c r="AT4" s="39"/>
-      <c r="AU4" s="39"/>
-      <c r="AV4" s="39"/>
-      <c r="AW4" s="40"/>
-      <c r="AX4" s="29"/>
-      <c r="AY4" s="41" t="s">
+      <c r="AR4" s="67"/>
+      <c r="AS4" s="68"/>
+      <c r="AT4" s="68"/>
+      <c r="AU4" s="68"/>
+      <c r="AV4" s="68"/>
+      <c r="AW4" s="69"/>
+      <c r="AX4" s="52"/>
+      <c r="AY4" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AZ4" s="41" t="s">
+      <c r="AZ4" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="BA4" s="41" t="s">
+      <c r="BA4" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="BB4" s="41" t="s">
+      <c r="BB4" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="BC4" s="41" t="s">
+      <c r="BC4" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="BD4" s="41" t="s">
+      <c r="BD4" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="BE4" s="29"/>
-      <c r="BF4" s="42" t="s">
+      <c r="BE4" s="52"/>
+      <c r="BF4" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="BG4" s="42" t="s">
+      <c r="BG4" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="BH4" s="42" t="s">
+      <c r="BH4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="BI4" s="43" t="s">
+      <c r="BI4" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="BJ4" s="42" t="s">
+      <c r="BJ4" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="BK4" s="44"/>
+      <c r="BK4" s="20"/>
     </row>
-    <row r="5" spans="1:63" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
-      <c r="B5" s="45">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.2">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21">
         <v>1</v>
       </c>
-      <c r="C5" s="45">
+      <c r="C5" s="21">
         <f t="shared" ref="C5:BD5" si="0">B5+1</f>
         <v>2</v>
       </c>
-      <c r="D5" s="45">
+      <c r="D5" s="21">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E5" s="45">
+      <c r="E5" s="21">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F5" s="45">
+      <c r="F5" s="21">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="45">
+      <c r="G5" s="21">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H5" s="45">
+      <c r="H5" s="21">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I5" s="45">
+      <c r="I5" s="21">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J5" s="45">
+      <c r="J5" s="21">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K5" s="45">
+      <c r="K5" s="21">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="L5" s="45">
+      <c r="L5" s="21">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="M5" s="45">
+      <c r="M5" s="21">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="N5" s="45">
+      <c r="N5" s="21">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="O5" s="45">
+      <c r="O5" s="21">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="P5" s="45">
+      <c r="P5" s="21">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="Q5" s="45">
+      <c r="Q5" s="21">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="R5" s="45">
+      <c r="R5" s="21">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="S5" s="45">
+      <c r="S5" s="21">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="T5" s="45">
+      <c r="T5" s="21">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="U5" s="45">
+      <c r="U5" s="21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="V5" s="45">
+      <c r="V5" s="21">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="W5" s="45">
+      <c r="W5" s="21">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="X5" s="45">
+      <c r="X5" s="21">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="Y5" s="45">
+      <c r="Y5" s="21">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="Z5" s="45">
+      <c r="Z5" s="21">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="AA5" s="45">
+      <c r="AA5" s="21">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="AB5" s="45">
+      <c r="AB5" s="21">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="AC5" s="45">
+      <c r="AC5" s="21">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="AD5" s="45">
+      <c r="AD5" s="21">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="AE5" s="45">
+      <c r="AE5" s="21">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AF5" s="45">
+      <c r="AF5" s="21">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AG5" s="45">
+      <c r="AG5" s="21">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="AH5" s="45">
+      <c r="AH5" s="21">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="AI5" s="45">
+      <c r="AI5" s="21">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="AJ5" s="45">
+      <c r="AJ5" s="21">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="AK5" s="45">
+      <c r="AK5" s="21">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="AL5" s="45">
+      <c r="AL5" s="21">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="AM5" s="45">
+      <c r="AM5" s="21">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="AN5" s="45">
+      <c r="AN5" s="21">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="AO5" s="45">
+      <c r="AO5" s="21">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="AP5" s="45">
+      <c r="AP5" s="21">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="AQ5" s="45">
+      <c r="AQ5" s="21">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="AR5" s="45">
+      <c r="AR5" s="21">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="AS5" s="45">
+      <c r="AS5" s="21">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="AT5" s="45">
+      <c r="AT5" s="21">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="AU5" s="45">
+      <c r="AU5" s="21">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="AV5" s="45">
+      <c r="AV5" s="21">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="AW5" s="45">
+      <c r="AW5" s="21">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="AX5" s="45">
+      <c r="AX5" s="21">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="AY5" s="45">
+      <c r="AY5" s="21">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="AZ5" s="45">
+      <c r="AZ5" s="21">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="BA5" s="45">
+      <c r="BA5" s="21">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="BB5" s="45">
+      <c r="BB5" s="21">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="BC5" s="45">
+      <c r="BC5" s="21">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="BD5" s="45">
+      <c r="BD5" s="21">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="BE5" s="46"/>
-      <c r="BF5" s="46"/>
-      <c r="BG5" s="46"/>
-      <c r="BH5" s="46"/>
-      <c r="BI5" s="47"/>
-      <c r="BJ5" s="46"/>
-      <c r="BK5" s="47"/>
+      <c r="BE5" s="22"/>
+      <c r="BF5" s="22"/>
+      <c r="BG5" s="22"/>
+      <c r="BH5" s="22"/>
+      <c r="BI5" s="23"/>
+      <c r="BJ5" s="22"/>
+      <c r="BK5" s="23"/>
     </row>
-    <row r="6" spans="1:63" s="9" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" ht="70" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>13</v>
       </c>
@@ -2468,67 +2317,67 @@
         <v>10700000</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E6" s="4">
         <v>30047</v>
       </c>
-      <c r="F6" s="50" t="s">
-        <v>168</v>
+      <c r="F6" s="25" t="s">
+        <v>182</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>145</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>58</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M6" s="2">
         <v>20767757</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>86</v>
       </c>
       <c r="P6" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="R6" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="Q6" s="5" t="s">
+      <c r="S6" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="R6" s="5" t="s">
+      <c r="T6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="V6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Y6" s="4">
         <v>44302</v>
@@ -2538,13 +2387,13 @@
         <v>44362</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AB6" s="5" t="s">
         <v>2</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AD6" s="4">
         <v>44363</v>
@@ -2553,13 +2402,13 @@
         <v>44727</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AG6" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AH6" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AI6" s="4">
         <v>44728</v>
@@ -2568,32 +2417,32 @@
         <v>45458</v>
       </c>
       <c r="AK6" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AL6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AM6" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="AL6" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AM6" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="AN6" s="4">
         <v>45459</v>
       </c>
       <c r="AO6" s="2"/>
       <c r="AP6" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AQ6" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AR6" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="AQ6" s="2" t="s">
+      <c r="AS6" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="AR6" s="2" t="s">
+      <c r="AT6" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="AS6" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="AT6" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="AU6" s="2"/>
       <c r="AV6" s="2"/>
@@ -2633,11 +2482,11 @@
         <v>44302</v>
       </c>
       <c r="BJ6" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BK6" s="8"/>
     </row>
-    <row r="7" spans="1:63" s="9" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" ht="84" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -2653,8 +2502,8 @@
       <c r="E7" s="4">
         <v>32484</v>
       </c>
-      <c r="F7" s="50" t="s">
-        <v>90</v>
+      <c r="F7" s="25" t="s">
+        <v>183</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>55</v>
@@ -2776,80 +2625,80 @@
       <c r="BJ7" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="BK7" s="48"/>
+      <c r="BK7" s="24"/>
     </row>
-    <row r="8" spans="1:63" s="9" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" ht="70" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C8" s="3">
         <v>6000000</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E8" s="4">
         <v>36285</v>
       </c>
-      <c r="F8" s="50" t="s">
-        <v>185</v>
-      </c>
-      <c r="G8" s="82" t="s">
+      <c r="F8" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="G8" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="K8" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="L8" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="M8" s="2">
         <v>111100012770007</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="Q8" s="5" t="s">
         <v>63</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="T8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="V8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="Y8" s="4">
         <v>45873</v>
@@ -2858,13 +2707,13 @@
         <v>45934</v>
       </c>
       <c r="AA8" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AB8" s="5" t="s">
         <v>2</v>
       </c>
       <c r="AC8" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AD8" s="4">
         <v>45935</v>
@@ -2873,10 +2722,10 @@
         <v>46299</v>
       </c>
       <c r="AF8" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="AG8" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
@@ -2933,7 +2782,7 @@
       </c>
       <c r="BK8" s="8"/>
     </row>
-    <row r="9" spans="1:63" s="9" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" ht="98" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>4</v>
       </c>
@@ -2949,8 +2798,8 @@
       <c r="E9" s="4">
         <v>33145</v>
       </c>
-      <c r="F9" s="50" t="s">
-        <v>91</v>
+      <c r="F9" s="25" t="s">
+        <v>185</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>74</v>
@@ -3083,6 +2932,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
     <mergeCell ref="AX3:AX4"/>
     <mergeCell ref="AY3:BD3"/>
     <mergeCell ref="BE3:BE4"/>
@@ -3099,95 +2961,46 @@
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
   </mergeCells>
-  <conditionalFormatting sqref="A7 C7:N7 P7:BK7">
-    <cfRule type="expression" dxfId="16" priority="12">
-      <formula>OR($T7="Đã nghỉ việc", $T7="Tạm dừng")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9 C9:N9 P9:BK9">
-    <cfRule type="expression" dxfId="14" priority="10">
-      <formula>OR($T9="Đã nghỉ việc", $T9="Tạm dừng")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="13" priority="9">
-      <formula>OR($T7="Đã nghỉ việc", $T7="Tạm dừng")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="expression" dxfId="11" priority="7">
-      <formula>OR($T9="Đã nghỉ việc", $T9="Tạm dừng")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O7">
-    <cfRule type="expression" dxfId="9" priority="5">
-      <formula>OR($T7="Đã nghỉ việc", $T7="Tạm dừng")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O9">
-    <cfRule type="expression" dxfId="7" priority="3">
-      <formula>OR($T9="Đã nghỉ việc", $T9="Tạm dừng")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A6:BK6">
-    <cfRule type="expression" dxfId="6" priority="2">
+  <conditionalFormatting sqref="A6:BK9">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>OR($T6="Đã nghỉ việc", $T6="Tạm dừng")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:BK8">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>OR($T8="Đã nghỉ việc", $T8="Tạm dừng")</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I4:I9 E6:E9">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I4:I9 E6:E9" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>OR(NOT(ISERROR(DATEVALUE(E4))), AND(ISNUMBER(E4), LEFT(CELL("format", E4))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="BF6:BF9">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="BF6:BF9" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Nam ,Nữ"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="T6:T9">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="T6:T9" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Đang làm việc,Đã nghỉ việc,Tạm dừng,Thai sản"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày hợp lệ" sqref="BI6:BI7 BE6:BE9 AD6:AE9">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày hợp lệ" sqref="BI6:BI7 BE6:BE9 AD6:AE9" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>OR(NOT(ISERROR(DATEVALUE(AD6))), AND(ISNUMBER(AD6), LEFT(CELL("format", AD6))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="V6:V9">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="V6:V9" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"Full-time,Part-time,CTV"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="U6:U9">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="U6:U9" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Chính thức,Thử việc,Dịch vụ,Khoán việc"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="BJ6:BJ9">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="BJ6:BJ9" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"HCNS,Tài chính,Vận hành VP,Vận hành Kho,Marketing ,Lãnh đạo,Kỹ thuật,Thiết kế"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F7" r:id="rId1"/>
-    <hyperlink ref="F9" r:id="rId2"/>
-    <hyperlink ref="F6" r:id="rId3"/>
-    <hyperlink ref="F8" r:id="rId4"/>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000007000000}">
           <x14:formula1>
             <xm:f>'[File mẫu.xlsx]Thiết lập'!#REF!</xm:f>
           </x14:formula1>
@@ -3200,1172 +3013,1167 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A1" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="77" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="78" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="79" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="82" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="56" t="s">
+      <c r="R1" s="80"/>
+      <c r="S1" s="80"/>
+      <c r="T1" s="81"/>
+      <c r="U1" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="57" t="s">
+      <c r="V1" s="80"/>
+      <c r="W1" s="80"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
+      <c r="Z1" s="80"/>
+      <c r="AA1" s="80"/>
+      <c r="AB1" s="80"/>
+      <c r="AC1" s="80"/>
+      <c r="AD1" s="80"/>
+      <c r="AE1" s="80"/>
+      <c r="AF1" s="80"/>
+      <c r="AG1" s="80"/>
+      <c r="AH1" s="81"/>
+      <c r="AI1" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="58" t="s">
+      <c r="AJ1" s="80"/>
+      <c r="AK1" s="80"/>
+      <c r="AL1" s="81"/>
+      <c r="AM1" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="55"/>
-      <c r="AI1" s="56" t="s">
+      <c r="AN1" s="81"/>
+      <c r="AO1" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="55"/>
-      <c r="AM1" s="59" t="s">
+      <c r="AP1" s="80"/>
+      <c r="AQ1" s="80"/>
+      <c r="AR1" s="80"/>
+      <c r="AS1" s="81"/>
+      <c r="AT1" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="AN1" s="55"/>
-      <c r="AO1" s="60" t="s">
+      <c r="AU1" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="55"/>
-      <c r="AT1" s="61" t="s">
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="26"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="26"/>
+      <c r="AZ1" s="26"/>
+      <c r="BA1" s="26"/>
+    </row>
+    <row r="2" spans="1:53" ht="140" x14ac:dyDescent="0.2">
+      <c r="A2" s="76"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="AU1" s="62" t="s">
+      <c r="E2" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="AV1" s="63"/>
-      <c r="AW1" s="63"/>
-      <c r="AX1" s="63"/>
-      <c r="AY1" s="63"/>
-      <c r="AZ1" s="63"/>
-      <c r="BA1" s="63"/>
+      <c r="F2" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="N2" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="O2" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="P2" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q2" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="R2" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="S2" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="T2" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="U2" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="V2" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="W2" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="X2" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y2" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z2" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA2" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB2" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC2" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD2" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE2" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="AF2" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="AG2" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="AH2" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI2" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ2" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="AK2" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="AL2" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="AM2" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="AN2" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="AO2" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP2" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="AQ2" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="AR2" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="AS2" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="AT2" s="76"/>
+      <c r="AU2" s="76"/>
+      <c r="AV2" s="26"/>
+      <c r="AW2" s="26"/>
+      <c r="AX2" s="26"/>
+      <c r="AY2" s="26"/>
+      <c r="AZ2" s="26"/>
+      <c r="BA2" s="26"/>
     </row>
-    <row r="2" spans="1:53" s="9" customFormat="1" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="64"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65" t="s">
-        <v>103</v>
-      </c>
-      <c r="E2" s="66" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2" s="67" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" s="66" t="s">
-        <v>106</v>
-      </c>
-      <c r="H2" s="67" t="s">
-        <v>107</v>
-      </c>
-      <c r="I2" s="67" t="s">
-        <v>108</v>
-      </c>
-      <c r="J2" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="K2" s="67" t="s">
-        <v>110</v>
-      </c>
-      <c r="L2" s="66" t="s">
-        <v>111</v>
-      </c>
-      <c r="M2" s="68" t="s">
-        <v>112</v>
-      </c>
-      <c r="N2" s="68" t="s">
-        <v>113</v>
-      </c>
-      <c r="O2" s="68" t="s">
-        <v>114</v>
-      </c>
-      <c r="P2" s="68" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q2" s="69" t="s">
-        <v>116</v>
-      </c>
-      <c r="R2" s="69" t="s">
-        <v>117</v>
-      </c>
-      <c r="S2" s="69" t="s">
-        <v>118</v>
-      </c>
-      <c r="T2" s="69" t="s">
-        <v>119</v>
-      </c>
-      <c r="U2" s="70" t="s">
-        <v>120</v>
-      </c>
-      <c r="V2" s="70" t="s">
-        <v>121</v>
-      </c>
-      <c r="W2" s="70" t="s">
-        <v>122</v>
-      </c>
-      <c r="X2" s="70" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y2" s="70" t="s">
-        <v>124</v>
-      </c>
-      <c r="Z2" s="70" t="s">
-        <v>125</v>
-      </c>
-      <c r="AA2" s="70" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB2" s="70" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC2" s="70" t="s">
-        <v>128</v>
-      </c>
-      <c r="AD2" s="70" t="s">
-        <v>129</v>
-      </c>
-      <c r="AE2" s="70" t="s">
-        <v>130</v>
-      </c>
-      <c r="AF2" s="70" t="s">
-        <v>131</v>
-      </c>
-      <c r="AG2" s="70" t="s">
-        <v>132</v>
-      </c>
-      <c r="AH2" s="70" t="s">
-        <v>133</v>
-      </c>
-      <c r="AI2" s="68" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ2" s="68" t="s">
-        <v>134</v>
-      </c>
-      <c r="AK2" s="68" t="s">
-        <v>135</v>
-      </c>
-      <c r="AL2" s="68" t="s">
-        <v>136</v>
-      </c>
-      <c r="AM2" s="71" t="s">
-        <v>99</v>
-      </c>
-      <c r="AN2" s="71" t="s">
-        <v>137</v>
-      </c>
-      <c r="AO2" s="72" t="s">
-        <v>116</v>
-      </c>
-      <c r="AP2" s="69" t="s">
-        <v>138</v>
-      </c>
-      <c r="AQ2" s="69" t="s">
-        <v>139</v>
-      </c>
-      <c r="AR2" s="72" t="s">
-        <v>140</v>
-      </c>
-      <c r="AS2" s="69" t="s">
-        <v>141</v>
-      </c>
-      <c r="AT2" s="64"/>
-      <c r="AU2" s="64"/>
-      <c r="AV2" s="63"/>
-      <c r="AW2" s="63"/>
-      <c r="AX2" s="63"/>
-      <c r="AY2" s="63"/>
-      <c r="AZ2" s="63"/>
-      <c r="BA2" s="63"/>
-    </row>
-    <row r="3" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="84"/>
-      <c r="B3" s="85" t="s">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A3" s="46"/>
+      <c r="B3" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="85">
+      <c r="C3" s="47">
         <f t="shared" ref="C3:AU3" si="0">B3+1</f>
         <v>2</v>
       </c>
-      <c r="D3" s="85">
+      <c r="D3" s="47">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E3" s="85">
+      <c r="E3" s="47">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F3" s="85">
+      <c r="F3" s="47">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G3" s="85">
+      <c r="G3" s="47">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H3" s="85">
+      <c r="H3" s="47">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I3" s="85">
+      <c r="I3" s="47">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J3" s="73">
+      <c r="J3" s="35">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K3" s="73">
+      <c r="K3" s="35">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="L3" s="73">
+      <c r="L3" s="35">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="M3" s="73">
+      <c r="M3" s="35">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="N3" s="73">
+      <c r="N3" s="35">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="O3" s="73">
+      <c r="O3" s="35">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="P3" s="73">
+      <c r="P3" s="35">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="Q3" s="73">
+      <c r="Q3" s="35">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="R3" s="73">
+      <c r="R3" s="35">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="S3" s="73">
+      <c r="S3" s="35">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="T3" s="73">
+      <c r="T3" s="35">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="U3" s="73">
+      <c r="U3" s="35">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="V3" s="73">
+      <c r="V3" s="35">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="W3" s="73">
+      <c r="W3" s="35">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="X3" s="73">
+      <c r="X3" s="35">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="Y3" s="73">
+      <c r="Y3" s="35">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="Z3" s="73">
+      <c r="Z3" s="35">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="AA3" s="73">
+      <c r="AA3" s="35">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="AB3" s="73">
+      <c r="AB3" s="35">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="AC3" s="73">
+      <c r="AC3" s="35">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="AD3" s="73">
+      <c r="AD3" s="35">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="AE3" s="73">
+      <c r="AE3" s="35">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AF3" s="73">
+      <c r="AF3" s="35">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AG3" s="73">
+      <c r="AG3" s="35">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="AH3" s="73">
+      <c r="AH3" s="35">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="AI3" s="73">
+      <c r="AI3" s="35">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="AJ3" s="73">
+      <c r="AJ3" s="35">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="AK3" s="73">
+      <c r="AK3" s="35">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="AL3" s="73">
+      <c r="AL3" s="35">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="AM3" s="73">
+      <c r="AM3" s="35">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="AN3" s="73">
+      <c r="AN3" s="35">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="AO3" s="73">
+      <c r="AO3" s="35">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="AP3" s="73">
+      <c r="AP3" s="35">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="AQ3" s="73">
+      <c r="AQ3" s="35">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="AR3" s="73">
+      <c r="AR3" s="35">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="AS3" s="73">
+      <c r="AS3" s="35">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="AT3" s="73">
+      <c r="AT3" s="35">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="AU3" s="73">
+      <c r="AU3" s="35">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="AV3" s="74"/>
-      <c r="AW3" s="74"/>
-      <c r="AX3" s="74"/>
-      <c r="AY3" s="74"/>
-      <c r="AZ3" s="74"/>
-      <c r="BA3" s="74"/>
+      <c r="AV3" s="36"/>
+      <c r="AW3" s="36"/>
+      <c r="AX3" s="36"/>
+      <c r="AY3" s="36"/>
+      <c r="AZ3" s="36"/>
+      <c r="BA3" s="36"/>
     </row>
-    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="86">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A4" s="48">
         <v>1</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="48">
         <v>9000000</v>
       </c>
-      <c r="D4" s="88">
+      <c r="D4" s="50">
         <f t="shared" ref="D4:D7" si="1">SUM(E4:L4)</f>
         <v>10070750</v>
       </c>
-      <c r="E4" s="88">
+      <c r="E4" s="50">
         <v>2000000</v>
       </c>
-      <c r="F4" s="88">
+      <c r="F4" s="50">
         <v>1500000</v>
       </c>
-      <c r="G4" s="88">
+      <c r="G4" s="50">
         <v>1500000</v>
       </c>
-      <c r="H4" s="88">
-        <v>0</v>
-      </c>
-      <c r="I4" s="88">
-        <v>0</v>
-      </c>
-      <c r="J4" s="83">
+      <c r="H4" s="50">
+        <v>0</v>
+      </c>
+      <c r="I4" s="50">
+        <v>0</v>
+      </c>
+      <c r="J4" s="45">
         <v>4670750</v>
       </c>
-      <c r="K4" s="76">
-        <v>0</v>
-      </c>
-      <c r="L4" s="76">
+      <c r="K4" s="38">
+        <v>0</v>
+      </c>
+      <c r="L4" s="38">
         <v>400000</v>
       </c>
-      <c r="M4" s="75">
+      <c r="M4" s="37">
         <f t="shared" ref="M4:M7" si="2">SUM(O4:P4)</f>
         <v>11000000</v>
       </c>
-      <c r="N4" s="75">
+      <c r="N4" s="37">
         <f t="shared" ref="N4" si="3">IF(B4="",0,0)</f>
         <v>0</v>
       </c>
-      <c r="O4" s="75">
+      <c r="O4" s="37">
         <f t="shared" ref="O4:O7" si="4">IF(B4="",0,11000000)</f>
         <v>11000000</v>
       </c>
-      <c r="P4" s="75">
+      <c r="P4" s="37">
         <f t="shared" ref="P4:P7" si="5">N4*4400000</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="75">
+      <c r="Q4" s="37">
         <f t="shared" ref="Q4:Q7" si="6">SUM(R4:T4)</f>
         <v>945000</v>
       </c>
-      <c r="R4" s="75">
+      <c r="R4" s="37">
         <f t="shared" ref="R4:R7" si="7">C4*8%</f>
         <v>720000</v>
       </c>
-      <c r="S4" s="75">
+      <c r="S4" s="37">
         <f t="shared" ref="S4:S7" si="8">C4*1.5%</f>
         <v>135000</v>
       </c>
-      <c r="T4" s="75">
+      <c r="T4" s="37">
         <f t="shared" ref="T4:T7" si="9">C4*1%</f>
         <v>90000</v>
       </c>
-      <c r="U4" s="77">
+      <c r="U4" s="39">
         <f t="shared" ref="U4:U7" si="10">C4+D4</f>
         <v>19070750</v>
       </c>
-      <c r="V4" s="75">
+      <c r="V4" s="37">
         <f t="shared" ref="V4:V7" si="11">U4-J4</f>
         <v>14400000</v>
       </c>
-      <c r="W4" s="75">
+      <c r="W4" s="37">
         <f t="shared" ref="W4:W7" si="12">15%*V4</f>
         <v>2160000</v>
       </c>
-      <c r="X4" s="76">
+      <c r="X4" s="38">
         <f t="shared" ref="X4:X7" si="13">J4-W4</f>
         <v>2510750</v>
       </c>
-      <c r="Y4" s="76">
+      <c r="Y4" s="38">
         <f t="shared" ref="Y4:Y7" si="14">U4-X4-E4-G4-L4</f>
         <v>12660000</v>
       </c>
-      <c r="Z4" s="76">
+      <c r="Z4" s="38">
         <f t="shared" ref="Z4:Z7" si="15">IF(Y4-M4-Q4&lt;=0, 0, Y4-M4-Q4)</f>
         <v>715000</v>
       </c>
-      <c r="AA4" s="76">
+      <c r="AA4" s="38">
         <f t="shared" ref="AA4:AA7" si="16">IF(SUM(AB4:AG4)=0,"0",SUM(AB4:AG4))</f>
         <v>35750</v>
       </c>
-      <c r="AB4" s="76">
+      <c r="AB4" s="38">
         <f t="shared" ref="AB4:AB7" si="17">MAX(0, MIN($Z4, 5000000)) * 5%</f>
         <v>35750</v>
       </c>
-      <c r="AC4" s="76">
+      <c r="AC4" s="38">
         <f t="shared" ref="AC4:AC7" si="18">MAX(0, MIN($Z4 - 5000000, 5000000)) * 10%</f>
         <v>0</v>
       </c>
-      <c r="AD4" s="76">
+      <c r="AD4" s="38">
         <f t="shared" ref="AD4:AD7" si="19">MAX(0, MIN($Z4 - 10000000, 8000000)) * 15%</f>
         <v>0</v>
       </c>
-      <c r="AE4" s="76">
+      <c r="AE4" s="38">
         <f t="shared" ref="AE4:AE7" si="20">MAX(0, MIN($Z4 - 18000000, 14000000)) * 20%</f>
         <v>0</v>
       </c>
-      <c r="AF4" s="76">
+      <c r="AF4" s="38">
         <f t="shared" ref="AF4:AF7" si="21">MAX(0, MIN($Z4 - 32000000, 20000000)) * 25%</f>
         <v>0</v>
       </c>
-      <c r="AG4" s="75">
+      <c r="AG4" s="37">
         <f t="shared" ref="AG4:AG7" si="22">MAX(0, MIN($Z4 - 52000000, 28000000)) * 30%</f>
         <v>0</v>
       </c>
-      <c r="AH4" s="75">
+      <c r="AH4" s="37">
         <f t="shared" ref="AH4:AH7" si="23">MAX(0, $Z4 - 80000000) * 35%</f>
         <v>0</v>
       </c>
-      <c r="AI4" s="75">
+      <c r="AI4" s="37">
         <f t="shared" ref="AI4:AI7" si="24">SUM(AJ4:AL4)</f>
         <v>1935000</v>
       </c>
-      <c r="AJ4" s="75">
+      <c r="AJ4" s="37">
         <f t="shared" ref="AJ4:AJ7" si="25">C4*17.5%</f>
         <v>1575000</v>
       </c>
-      <c r="AK4" s="75">
+      <c r="AK4" s="37">
         <f t="shared" ref="AK4:AK7" si="26">C4*1%</f>
         <v>90000</v>
       </c>
-      <c r="AL4" s="75">
+      <c r="AL4" s="37">
         <f t="shared" ref="AL4:AL7" si="27">C4*3%</f>
         <v>270000</v>
       </c>
-      <c r="AM4" s="76">
+      <c r="AM4" s="38">
         <f t="shared" ref="AM4:AM7" si="28">C4*2%</f>
         <v>180000</v>
       </c>
-      <c r="AN4" s="76">
+      <c r="AN4" s="38">
         <f t="shared" ref="AN4:AN7" si="29">C4*1%</f>
         <v>90000</v>
       </c>
-      <c r="AO4" s="78">
+      <c r="AO4" s="40">
         <f t="shared" ref="AO4:AO7" si="30">SUM(AP4:AS4)</f>
         <v>3095750</v>
       </c>
-      <c r="AP4" s="75">
+      <c r="AP4" s="37">
         <f t="shared" ref="AP4:AP7" si="31">Q4</f>
         <v>945000</v>
       </c>
-      <c r="AQ4" s="75">
+      <c r="AQ4" s="37">
         <f t="shared" ref="AQ4:AQ7" si="32">AA4</f>
         <v>35750</v>
       </c>
-      <c r="AR4" s="75">
+      <c r="AR4" s="37">
         <f t="shared" ref="AR4:AR7" si="33">AI4</f>
         <v>1935000</v>
       </c>
-      <c r="AS4" s="75">
+      <c r="AS4" s="37">
         <f t="shared" ref="AS4:AS7" si="34">AM4</f>
         <v>180000</v>
       </c>
-      <c r="AT4" s="75">
+      <c r="AT4" s="37">
         <f t="shared" ref="AT4:AT7" si="35">U4-Q4-AA4-AN4</f>
         <v>18000000</v>
       </c>
-      <c r="AU4" s="75">
+      <c r="AU4" s="37">
         <f t="shared" ref="AU4:AU7" si="36">AT4+AO4</f>
         <v>21095750</v>
       </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="79"/>
+      <c r="AV4" s="41"/>
+      <c r="AW4" s="41"/>
+      <c r="AX4" s="41"/>
+      <c r="AY4" s="41"/>
+      <c r="AZ4" s="41"/>
+      <c r="BA4" s="41"/>
     </row>
-    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="86">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A5" s="48">
         <v>2</v>
       </c>
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="86">
+      <c r="C5" s="48">
         <v>22000000</v>
       </c>
-      <c r="D5" s="88">
+      <c r="D5" s="50">
         <f t="shared" si="1"/>
         <v>28000000</v>
       </c>
-      <c r="E5" s="88">
+      <c r="E5" s="50">
         <v>5000000</v>
       </c>
-      <c r="F5" s="88">
+      <c r="F5" s="50">
         <v>5000000</v>
       </c>
-      <c r="G5" s="88">
+      <c r="G5" s="50">
         <v>2000000</v>
       </c>
-      <c r="H5" s="88">
-        <v>0</v>
-      </c>
-      <c r="I5" s="88">
-        <v>0</v>
-      </c>
-      <c r="J5" s="83">
+      <c r="H5" s="50">
+        <v>0</v>
+      </c>
+      <c r="I5" s="50">
+        <v>0</v>
+      </c>
+      <c r="J5" s="45">
         <v>15600000</v>
       </c>
-      <c r="K5" s="76">
-        <v>0</v>
-      </c>
-      <c r="L5" s="76">
+      <c r="K5" s="38">
+        <v>0</v>
+      </c>
+      <c r="L5" s="38">
         <v>400000</v>
       </c>
-      <c r="M5" s="75">
+      <c r="M5" s="37">
         <f t="shared" si="2"/>
         <v>15400000</v>
       </c>
-      <c r="N5" s="75">
+      <c r="N5" s="37">
         <v>1</v>
       </c>
-      <c r="O5" s="75">
+      <c r="O5" s="37">
         <f t="shared" si="4"/>
         <v>11000000</v>
       </c>
-      <c r="P5" s="75">
+      <c r="P5" s="37">
         <f t="shared" si="5"/>
         <v>4400000</v>
       </c>
-      <c r="Q5" s="75">
+      <c r="Q5" s="37">
         <f t="shared" si="6"/>
         <v>2310000</v>
       </c>
-      <c r="R5" s="75">
+      <c r="R5" s="37">
         <f t="shared" si="7"/>
         <v>1760000</v>
       </c>
-      <c r="S5" s="75">
+      <c r="S5" s="37">
         <f t="shared" si="8"/>
         <v>330000</v>
       </c>
-      <c r="T5" s="75">
+      <c r="T5" s="37">
         <f t="shared" si="9"/>
         <v>220000</v>
       </c>
-      <c r="U5" s="77">
+      <c r="U5" s="39">
         <f t="shared" si="10"/>
         <v>50000000</v>
       </c>
-      <c r="V5" s="75">
+      <c r="V5" s="37">
         <f t="shared" si="11"/>
         <v>34400000</v>
       </c>
-      <c r="W5" s="75">
+      <c r="W5" s="37">
         <f t="shared" si="12"/>
         <v>5160000</v>
       </c>
-      <c r="X5" s="76">
+      <c r="X5" s="38">
         <f t="shared" si="13"/>
         <v>10440000</v>
       </c>
-      <c r="Y5" s="76">
+      <c r="Y5" s="38">
         <f t="shared" si="14"/>
         <v>32160000</v>
       </c>
-      <c r="Z5" s="76">
+      <c r="Z5" s="38">
         <f t="shared" si="15"/>
         <v>14450000</v>
       </c>
-      <c r="AA5" s="76">
+      <c r="AA5" s="38">
         <f t="shared" si="16"/>
         <v>1417500</v>
       </c>
-      <c r="AB5" s="76">
+      <c r="AB5" s="38">
         <f t="shared" si="17"/>
         <v>250000</v>
       </c>
-      <c r="AC5" s="76">
+      <c r="AC5" s="38">
         <f t="shared" si="18"/>
         <v>500000</v>
       </c>
-      <c r="AD5" s="76">
+      <c r="AD5" s="38">
         <f t="shared" si="19"/>
         <v>667500</v>
       </c>
-      <c r="AE5" s="76">
+      <c r="AE5" s="38">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="AF5" s="76">
+      <c r="AF5" s="38">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AG5" s="75">
+      <c r="AG5" s="37">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="AH5" s="75">
+      <c r="AH5" s="37">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AI5" s="75">
+      <c r="AI5" s="37">
         <f t="shared" si="24"/>
         <v>4730000</v>
       </c>
-      <c r="AJ5" s="75">
+      <c r="AJ5" s="37">
         <f t="shared" si="25"/>
         <v>3849999.9999999995</v>
       </c>
-      <c r="AK5" s="75">
+      <c r="AK5" s="37">
         <f t="shared" si="26"/>
         <v>220000</v>
       </c>
-      <c r="AL5" s="75">
+      <c r="AL5" s="37">
         <f t="shared" si="27"/>
         <v>660000</v>
       </c>
-      <c r="AM5" s="76">
+      <c r="AM5" s="38">
         <f t="shared" si="28"/>
         <v>440000</v>
       </c>
-      <c r="AN5" s="76">
+      <c r="AN5" s="38">
         <f t="shared" si="29"/>
         <v>220000</v>
       </c>
-      <c r="AO5" s="78">
+      <c r="AO5" s="40">
         <f t="shared" si="30"/>
         <v>8897500</v>
       </c>
-      <c r="AP5" s="75">
+      <c r="AP5" s="37">
         <f t="shared" si="31"/>
         <v>2310000</v>
       </c>
-      <c r="AQ5" s="75">
+      <c r="AQ5" s="37">
         <f t="shared" si="32"/>
         <v>1417500</v>
       </c>
-      <c r="AR5" s="75">
+      <c r="AR5" s="37">
         <f t="shared" si="33"/>
         <v>4730000</v>
       </c>
-      <c r="AS5" s="75">
+      <c r="AS5" s="37">
         <f t="shared" si="34"/>
         <v>440000</v>
       </c>
-      <c r="AT5" s="75">
+      <c r="AT5" s="37">
         <f t="shared" si="35"/>
         <v>46052500</v>
       </c>
-      <c r="AU5" s="75">
+      <c r="AU5" s="37">
         <f t="shared" si="36"/>
         <v>54950000</v>
       </c>
-      <c r="AV5" s="80"/>
-      <c r="AW5" s="80"/>
-      <c r="AX5" s="80"/>
-      <c r="AY5" s="80"/>
-      <c r="AZ5" s="80"/>
-      <c r="BA5" s="80"/>
+      <c r="AV5" s="42"/>
+      <c r="AW5" s="42"/>
+      <c r="AX5" s="42"/>
+      <c r="AY5" s="42"/>
+      <c r="AZ5" s="42"/>
+      <c r="BA5" s="42"/>
     </row>
-    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="86">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A6" s="48">
         <v>3</v>
       </c>
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="86">
+      <c r="C6" s="48">
         <v>10700000</v>
       </c>
-      <c r="D6" s="88">
+      <c r="D6" s="50">
         <f t="shared" si="1"/>
         <v>26400000</v>
       </c>
-      <c r="E6" s="88">
+      <c r="E6" s="50">
         <v>4000000</v>
       </c>
-      <c r="F6" s="88">
+      <c r="F6" s="50">
         <v>2000000</v>
       </c>
-      <c r="G6" s="88">
+      <c r="G6" s="50">
         <v>2000000</v>
       </c>
-      <c r="H6" s="88">
-        <v>0</v>
-      </c>
-      <c r="I6" s="88">
-        <v>0</v>
-      </c>
-      <c r="J6" s="83">
+      <c r="H6" s="50">
+        <v>0</v>
+      </c>
+      <c r="I6" s="50">
+        <v>0</v>
+      </c>
+      <c r="J6" s="45">
         <v>18000000</v>
       </c>
-      <c r="K6" s="76">
-        <v>0</v>
-      </c>
-      <c r="L6" s="76">
+      <c r="K6" s="38">
+        <v>0</v>
+      </c>
+      <c r="L6" s="38">
         <v>400000</v>
       </c>
-      <c r="M6" s="75">
+      <c r="M6" s="37">
         <f t="shared" si="2"/>
         <v>19800000</v>
       </c>
-      <c r="N6" s="75">
+      <c r="N6" s="37">
         <v>2</v>
       </c>
-      <c r="O6" s="75">
+      <c r="O6" s="37">
         <f t="shared" si="4"/>
         <v>11000000</v>
       </c>
-      <c r="P6" s="75">
+      <c r="P6" s="37">
         <f t="shared" si="5"/>
         <v>8800000</v>
       </c>
-      <c r="Q6" s="75">
+      <c r="Q6" s="37">
         <f t="shared" si="6"/>
         <v>1123500</v>
       </c>
-      <c r="R6" s="75">
+      <c r="R6" s="37">
         <f t="shared" si="7"/>
         <v>856000</v>
       </c>
-      <c r="S6" s="75">
+      <c r="S6" s="37">
         <f t="shared" si="8"/>
         <v>160500</v>
       </c>
-      <c r="T6" s="75">
+      <c r="T6" s="37">
         <f t="shared" si="9"/>
         <v>107000</v>
       </c>
-      <c r="U6" s="77">
+      <c r="U6" s="39">
         <f t="shared" si="10"/>
         <v>37100000</v>
       </c>
-      <c r="V6" s="75">
+      <c r="V6" s="37">
         <f t="shared" si="11"/>
         <v>19100000</v>
       </c>
-      <c r="W6" s="75">
+      <c r="W6" s="37">
         <f t="shared" si="12"/>
         <v>2865000</v>
       </c>
-      <c r="X6" s="76">
+      <c r="X6" s="38">
         <f t="shared" si="13"/>
         <v>15135000</v>
       </c>
-      <c r="Y6" s="76">
+      <c r="Y6" s="38">
         <f t="shared" si="14"/>
         <v>15565000</v>
       </c>
-      <c r="Z6" s="76">
+      <c r="Z6" s="38">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AA6" s="76" t="str">
+      <c r="AA6" s="38" t="str">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AB6" s="76">
+      <c r="AB6" s="38">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AC6" s="76">
+      <c r="AC6" s="38">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="AD6" s="76">
+      <c r="AD6" s="38">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="AE6" s="76">
+      <c r="AE6" s="38">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="AF6" s="76">
+      <c r="AF6" s="38">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AG6" s="75">
+      <c r="AG6" s="37">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="AH6" s="75">
+      <c r="AH6" s="37">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AI6" s="75">
+      <c r="AI6" s="37">
         <f t="shared" si="24"/>
         <v>2300500</v>
       </c>
-      <c r="AJ6" s="75">
+      <c r="AJ6" s="37">
         <f t="shared" si="25"/>
         <v>1872499.9999999998</v>
       </c>
-      <c r="AK6" s="75">
+      <c r="AK6" s="37">
         <f t="shared" si="26"/>
         <v>107000</v>
       </c>
-      <c r="AL6" s="75">
+      <c r="AL6" s="37">
         <f t="shared" si="27"/>
         <v>321000</v>
       </c>
-      <c r="AM6" s="76">
+      <c r="AM6" s="38">
         <f t="shared" si="28"/>
         <v>214000</v>
       </c>
-      <c r="AN6" s="76">
+      <c r="AN6" s="38">
         <f t="shared" si="29"/>
         <v>107000</v>
       </c>
-      <c r="AO6" s="78">
+      <c r="AO6" s="40">
         <f t="shared" si="30"/>
         <v>3638000</v>
       </c>
-      <c r="AP6" s="75">
+      <c r="AP6" s="37">
         <f t="shared" si="31"/>
         <v>1123500</v>
       </c>
-      <c r="AQ6" s="75" t="str">
+      <c r="AQ6" s="37" t="str">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="AR6" s="75">
+      <c r="AR6" s="37">
         <f t="shared" si="33"/>
         <v>2300500</v>
       </c>
-      <c r="AS6" s="75">
+      <c r="AS6" s="37">
         <f t="shared" si="34"/>
         <v>214000</v>
       </c>
-      <c r="AT6" s="75">
+      <c r="AT6" s="37">
         <f t="shared" si="35"/>
         <v>35869500</v>
       </c>
-      <c r="AU6" s="75">
+      <c r="AU6" s="37">
         <f t="shared" si="36"/>
         <v>39507500</v>
       </c>
-      <c r="AV6" s="81"/>
-      <c r="AW6" s="81"/>
-      <c r="AX6" s="81"/>
-      <c r="AY6" s="81"/>
-      <c r="AZ6" s="81"/>
-      <c r="BA6" s="81"/>
+      <c r="AV6" s="43"/>
+      <c r="AW6" s="43"/>
+      <c r="AX6" s="43"/>
+      <c r="AY6" s="43"/>
+      <c r="AZ6" s="43"/>
+      <c r="BA6" s="43"/>
     </row>
-    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="86">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A7" s="48">
         <v>4</v>
       </c>
-      <c r="B7" s="87" t="s">
-        <v>184</v>
-      </c>
-      <c r="C7" s="86">
+      <c r="B7" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="48">
         <v>6000000</v>
       </c>
-      <c r="D7" s="88">
+      <c r="D7" s="50">
         <f t="shared" si="1"/>
         <v>6690000</v>
       </c>
-      <c r="E7" s="88">
+      <c r="E7" s="50">
         <v>1500000</v>
       </c>
-      <c r="F7" s="88">
+      <c r="F7" s="50">
         <v>1000000</v>
       </c>
-      <c r="G7" s="88">
+      <c r="G7" s="50">
         <v>1000000</v>
       </c>
-      <c r="H7" s="88">
-        <v>0</v>
-      </c>
-      <c r="I7" s="88">
-        <v>0</v>
-      </c>
-      <c r="J7" s="83">
+      <c r="H7" s="50">
+        <v>0</v>
+      </c>
+      <c r="I7" s="50">
+        <v>0</v>
+      </c>
+      <c r="J7" s="45">
         <v>2790000</v>
       </c>
-      <c r="K7" s="76">
-        <v>0</v>
-      </c>
-      <c r="L7" s="76">
+      <c r="K7" s="38">
+        <v>0</v>
+      </c>
+      <c r="L7" s="38">
         <v>400000</v>
       </c>
-      <c r="M7" s="75">
+      <c r="M7" s="37">
         <f t="shared" si="2"/>
         <v>11000000</v>
       </c>
-      <c r="N7" s="75">
-        <v>0</v>
-      </c>
-      <c r="O7" s="75">
+      <c r="N7" s="37">
+        <v>0</v>
+      </c>
+      <c r="O7" s="37">
         <f t="shared" si="4"/>
         <v>11000000</v>
       </c>
-      <c r="P7" s="75">
+      <c r="P7" s="37">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q7" s="75">
+      <c r="Q7" s="37">
         <f t="shared" si="6"/>
         <v>630000</v>
       </c>
-      <c r="R7" s="75">
+      <c r="R7" s="37">
         <f t="shared" si="7"/>
         <v>480000</v>
       </c>
-      <c r="S7" s="75">
+      <c r="S7" s="37">
         <f t="shared" si="8"/>
         <v>90000</v>
       </c>
-      <c r="T7" s="75">
+      <c r="T7" s="37">
         <f t="shared" si="9"/>
         <v>60000</v>
       </c>
-      <c r="U7" s="77">
+      <c r="U7" s="39">
         <f t="shared" si="10"/>
         <v>12690000</v>
       </c>
-      <c r="V7" s="75">
+      <c r="V7" s="37">
         <f t="shared" si="11"/>
         <v>9900000</v>
       </c>
-      <c r="W7" s="75">
+      <c r="W7" s="37">
         <f t="shared" si="12"/>
         <v>1485000</v>
       </c>
-      <c r="X7" s="76">
+      <c r="X7" s="38">
         <f t="shared" si="13"/>
         <v>1305000</v>
       </c>
-      <c r="Y7" s="76">
+      <c r="Y7" s="38">
         <f t="shared" si="14"/>
         <v>8485000</v>
       </c>
-      <c r="Z7" s="76">
+      <c r="Z7" s="38">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AA7" s="76" t="str">
+      <c r="AA7" s="38" t="str">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AB7" s="76">
+      <c r="AB7" s="38">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AC7" s="76">
+      <c r="AC7" s="38">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="AD7" s="76">
+      <c r="AD7" s="38">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="AE7" s="76">
+      <c r="AE7" s="38">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="AF7" s="76">
+      <c r="AF7" s="38">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AG7" s="75">
+      <c r="AG7" s="37">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="AH7" s="75">
+      <c r="AH7" s="37">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AI7" s="75">
+      <c r="AI7" s="37">
         <f t="shared" si="24"/>
         <v>1290000</v>
       </c>
-      <c r="AJ7" s="75">
+      <c r="AJ7" s="37">
         <f t="shared" si="25"/>
         <v>1050000</v>
       </c>
-      <c r="AK7" s="75">
+      <c r="AK7" s="37">
         <f t="shared" si="26"/>
         <v>60000</v>
       </c>
-      <c r="AL7" s="75">
+      <c r="AL7" s="37">
         <f t="shared" si="27"/>
         <v>180000</v>
       </c>
-      <c r="AM7" s="76">
+      <c r="AM7" s="38">
         <f t="shared" si="28"/>
         <v>120000</v>
       </c>
-      <c r="AN7" s="76">
+      <c r="AN7" s="38">
         <f t="shared" si="29"/>
         <v>60000</v>
       </c>
-      <c r="AO7" s="78">
+      <c r="AO7" s="40">
         <f t="shared" si="30"/>
         <v>2040000</v>
       </c>
-      <c r="AP7" s="75">
+      <c r="AP7" s="37">
         <f t="shared" si="31"/>
         <v>630000</v>
       </c>
-      <c r="AQ7" s="75" t="str">
+      <c r="AQ7" s="37" t="str">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="AR7" s="75">
+      <c r="AR7" s="37">
         <f t="shared" si="33"/>
         <v>1290000</v>
       </c>
-      <c r="AS7" s="75">
+      <c r="AS7" s="37">
         <f t="shared" si="34"/>
         <v>120000</v>
       </c>
-      <c r="AT7" s="75">
+      <c r="AT7" s="37">
         <f t="shared" si="35"/>
         <v>12000000</v>
       </c>
-      <c r="AU7" s="75">
+      <c r="AU7" s="37">
         <f t="shared" si="36"/>
         <v>14040000</v>
       </c>
-      <c r="AV7" s="80"/>
-      <c r="AW7" s="80"/>
-      <c r="AX7" s="80"/>
-      <c r="AY7" s="80"/>
-      <c r="AZ7" s="80"/>
-      <c r="BA7" s="80"/>
+      <c r="AV7" s="42"/>
+      <c r="AW7" s="42"/>
+      <c r="AX7" s="42"/>
+      <c r="AY7" s="42"/>
+      <c r="AZ7" s="42"/>
+      <c r="BA7" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="U1:AH1"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="AM1:AN1"/>
-    <mergeCell ref="AO1:AS1"/>
-    <mergeCell ref="AT1:AT2"/>
     <mergeCell ref="AU1:AU2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -4373,25 +4181,15 @@
     <mergeCell ref="D1:L1"/>
     <mergeCell ref="M1:P1"/>
     <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U1:AH1"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="AO1:AS1"/>
+    <mergeCell ref="AT1:AT2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="4" priority="4">
+  <conditionalFormatting sqref="B4:B7">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>OR($T4="Đã nghỉ việc", $T4="Tạm dừng")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>OR($T5="Đã nghỉ việc", $T5="Tạm dừng")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>OR($T6="Đã nghỉ việc", $T6="Tạm dừng")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>OR($T7="Đã nghỉ việc", $T7="Tạm dừng")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>